<commit_message>
docs loading into arango
</commit_message>
<xml_diff>
--- a/packages/arango/tests/test-arango-data-loading.xlsx
+++ b/packages/arango/tests/test-arango-data-loading.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/arango/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3D1E9-59C4-0D4F-8F3C-F65B6E75189C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6741BB-C562-1046-ACED-CB7CD3D978A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66700" yWindow="4200" windowWidth="30340" windowHeight="19240" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" activeTab="2" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="DocCollectionOne" sheetId="1" r:id="rId1"/>
-    <sheet name=".lists" sheetId="7" r:id="rId2"/>
+    <sheet name="DocCollectionTwo" sheetId="8" r:id="rId2"/>
+    <sheet name="DocCollectionThree" sheetId="9" r:id="rId3"/>
+    <sheet name=".lists" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="DataTypeList">'.lists'!$A$2:$A$8</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>passwordHash</t>
   </si>
@@ -144,6 +146,66 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>dc2-1</t>
+  </si>
+  <si>
+    <t>dc2-2</t>
+  </si>
+  <si>
+    <t>dc3-3</t>
+  </si>
+  <si>
+    <t>TEST_DOC</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>test-doc-1</t>
+  </si>
+  <si>
+    <t>test-doc-2</t>
+  </si>
+  <si>
+    <t>test-doc-3</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>createAt</t>
+  </si>
+  <si>
+    <t>graph-start-1</t>
+  </si>
+  <si>
+    <t>graph-start-2</t>
+  </si>
+  <si>
+    <t>graph-start-3</t>
+  </si>
+  <si>
+    <t>graph-intermediate-1</t>
+  </si>
+  <si>
+    <t>graph-intermediate-2</t>
+  </si>
+  <si>
+    <t>graph-intermediate-3</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Test all datatypes in arango DB. Docs in the collection served as starting nodes in our  test graph</t>
+  </si>
+  <si>
+    <t>Docs in the collection serve as intermediary nodes in our  test graph</t>
+  </si>
+  <si>
+    <t>Docs in the collection serve as terminating nodes in our  test graph</t>
   </si>
 </sst>
 </file>
@@ -552,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,12 +630,12 @@
     <col min="7" max="7" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -584,190 +646,216 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2">
         <v>88</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2" t="b">
+      <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="8">
+      <c r="F7" s="8">
         <v>40848</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="2">
         <v>99</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="b">
+      <c r="E8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="8">
+      <c r="F8" s="8">
         <v>41255</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2">
-        <v>111</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2">
+        <v>222</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="b">
+      <c r="E9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E8" s="8">
+      <c r="F9" s="8">
         <v>36892</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D9" s="3"/>
-      <c r="E9" s="8"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D10" s="3"/>
       <c r="E10" s="8"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
       <c r="E11" s="8"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="E12" s="11"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+      <c r="E12" s="8"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="E13" s="11"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="10"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="10"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:J5" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:H5 B2" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:I6 B2:B3" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{9D944A17-348B-2D41-9A48-E3B02CE6F37B}">
@@ -780,6 +868,366 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCF2433-1C26-0C43-8A34-52888F2E6BE4}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="21.6640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>44822</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{B161CFA1-135B-6D49-B5CC-F61B2F9AF6D2}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:E6 B2:B3" xr:uid="{BF2B3865-DF15-B24D-A601-878E83F24658}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G6" xr:uid="{E34B6D38-0ACC-7449-9411-B684E60C1323}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D69BDD-48F5-1245-8B3A-149AD4BE0AAC}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="21.6640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>44822</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G6" xr:uid="{41222D5A-5662-694F-844D-BE04CA29514E}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:E6 B2:B3" xr:uid="{5120B4F6-C601-3140-B7F8-CE6CDD60D0E4}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{76C32FC5-0C64-BE40-8599-8439B3EDEE26}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>

<commit_message>
edge collections added to test, better parsing error reporting
</commit_message>
<xml_diff>
--- a/packages/arango/tests/test-arango-data-loading.xlsx
+++ b/packages/arango/tests/test-arango-data-loading.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/arango/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6741BB-C562-1046-ACED-CB7CD3D978A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AAC8AE-4CC2-364B-9C03-DC274EEC1D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" activeTab="2" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="63120" yWindow="1320" windowWidth="24580" windowHeight="25620" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="DocCollectionOne" sheetId="1" r:id="rId1"/>
-    <sheet name="DocCollectionTwo" sheetId="8" r:id="rId2"/>
-    <sheet name="DocCollectionThree" sheetId="9" r:id="rId3"/>
-    <sheet name=".lists" sheetId="7" r:id="rId4"/>
+    <sheet name="DocCollection1" sheetId="1" r:id="rId1"/>
+    <sheet name="DocCollection2" sheetId="8" r:id="rId2"/>
+    <sheet name="DocCollection3" sheetId="9" r:id="rId3"/>
+    <sheet name="EdgeCollection1" sheetId="11" r:id="rId4"/>
+    <sheet name=".EdgeCollection2" sheetId="12" r:id="rId5"/>
+    <sheet name=".lists" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="DataTypeList">'.lists'!$A$2:$A$8</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
   <si>
     <t>passwordHash</t>
   </si>
@@ -157,21 +159,9 @@
     <t>dc3-3</t>
   </si>
   <si>
-    <t>TEST_DOC</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>test-doc-1</t>
-  </si>
-  <si>
-    <t>test-doc-2</t>
-  </si>
-  <si>
-    <t>test-doc-3</t>
-  </si>
-  <si>
     <t>valid</t>
   </si>
   <si>
@@ -206,6 +196,102 @@
   </si>
   <si>
     <t>Docs in the collection serve as terminating nodes in our  test graph</t>
+  </si>
+  <si>
+    <t>dc3-1</t>
+  </si>
+  <si>
+    <t>dc3-2</t>
+  </si>
+  <si>
+    <t>_from</t>
+  </si>
+  <si>
+    <t>_to</t>
+  </si>
+  <si>
+    <t>ec1-1</t>
+  </si>
+  <si>
+    <t>ec2-2</t>
+  </si>
+  <si>
+    <t>graph-terminate-1</t>
+  </si>
+  <si>
+    <t>graph-terminate-2</t>
+  </si>
+  <si>
+    <t>graph-terminate-3</t>
+  </si>
+  <si>
+    <t>G-MIDDLE</t>
+  </si>
+  <si>
+    <t>G-START</t>
+  </si>
+  <si>
+    <t>G-END</t>
+  </si>
+  <si>
+    <t>DocCollection1/dc1-1</t>
+  </si>
+  <si>
+    <t>G-LEG-1</t>
+  </si>
+  <si>
+    <t>Edges in the collection serve as  edges from collection1 to collection 2</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> type</t>
+  </si>
+  <si>
+    <t>ec2-1</t>
+  </si>
+  <si>
+    <t>ec1-2</t>
+  </si>
+  <si>
+    <t>ec1-3</t>
+  </si>
+  <si>
+    <t>ec2-3</t>
+  </si>
+  <si>
+    <t>ec2-4</t>
+  </si>
+  <si>
+    <t>ec2-5</t>
+  </si>
+  <si>
+    <t>G-LEG-2</t>
+  </si>
+  <si>
+    <t>DocCollection2/dc2-1</t>
+  </si>
+  <si>
+    <t>DocCollection2/dc2-2</t>
+  </si>
+  <si>
+    <t>DocCollection2/dc2-3</t>
+  </si>
+  <si>
+    <t>DocCollection3/dc3-1</t>
+  </si>
+  <si>
+    <t>DocCollection3/dc3-2</t>
+  </si>
+  <si>
+    <t>DocCollection3/dc3-3</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>C1D1 -&gt; C2*</t>
   </si>
 </sst>
 </file>
@@ -614,28 +700,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="21.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1"/>
+    <col min="1" max="3" width="15.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="21.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -646,52 +732,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -699,144 +788,156 @@
         <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="2">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2">
         <v>88</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="b">
+      <c r="F7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="8">
         <v>40848</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="2">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2">
         <v>99</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="2" t="b">
+      <c r="F8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="8">
+      <c r="G8" s="8">
         <v>41255</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="2">
+        <v>43</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2">
         <v>222</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="2" t="b">
+      <c r="F9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G9" s="8">
         <v>36892</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D10" s="3"/>
-      <c r="E10" s="8"/>
-      <c r="G10" s="2"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E10" s="3"/>
+      <c r="F10" s="8"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-      <c r="E11" s="8"/>
-      <c r="G11" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E11" s="3"/>
+      <c r="F11" s="8"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D12" s="3"/>
-      <c r="E12" s="8"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E12" s="3"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="E13" s="11"/>
-      <c r="G13" s="2"/>
+      <c r="D13" s="9"/>
+      <c r="F13" s="11"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D14" s="3"/>
-      <c r="G14" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14" s="3"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -844,18 +945,19 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D16" s="3"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="10"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:I6 B2:B3" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C3 A6:J6" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{9D944A17-348B-2D41-9A48-E3B02CE6F37B}">
@@ -872,7 +974,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -901,13 +1003,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -923,13 +1025,13 @@
         <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -954,10 +1056,10 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -971,10 +1073,10 @@
         <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
@@ -988,10 +1090,10 @@
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -1051,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D69BDD-48F5-1245-8B3A-149AD4BE0AAC}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,13 +1183,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1103,13 +1205,13 @@
         <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1131,36 +1233,36 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="8">
-        <v>45553</v>
+        <v>45554</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="8">
-        <v>45187</v>
+        <v>45554</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1168,16 +1270,16 @@
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="8">
-        <v>44822</v>
+        <v>45554</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1228,6 +1330,374 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6081FBB0-DD45-E143-A59A-BFD854210439}">
+  <dimension ref="A1:E1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="9"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="9"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="9"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="1048576" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E1048576" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{45421B7B-29D7-AC45-841A-41B842309904}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 A6:E6" xr:uid="{178F24EF-6D92-D545-8CE5-FA6A9C64728F}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6" xr:uid="{480E8F86-FB3B-364F-AE37-38E7D49BB503}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D611DF6E-379A-0F4C-A9ED-39C07B522875}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:F6" xr:uid="{FF2A09C6-3AF7-8140-A380-4475D17A1CAE}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 A6:D6" xr:uid="{0015496E-6437-F341-990B-EBAAB161F1C1}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{067EF2D7-458D-CB4F-847A-741EA0CDC7D2}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>

<commit_message>
56 add arango data loader continued (#76)
* docs loading into arango

* edge collections added to test, better parsing error reporting

* Add utils to check doc existance

* add validation for edge creation

* check point

* improve spreadsheet parser tests

* add data list parsing and tests

* Start string:list parsing

* better definition of data types

* change HorizDataLsit name -> HorizValueList

* checkpoint

* rename DataTypes to DataTypeMap and MetaTypes to MetaTypeMap

* change names propType(s) -> dataType(s)

* Finish row value parsing

* data list testing done

* add clean:all to a couple of packages
</commit_message>
<xml_diff>
--- a/packages/arango/tests/test-arango-data-loading.xlsx
+++ b/packages/arango/tests/test-arango-data-loading.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/arango/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3D1E9-59C4-0D4F-8F3C-F65B6E75189C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C45860A-DF59-7847-BA60-B9E1E7C6813C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66700" yWindow="4200" windowWidth="30340" windowHeight="19240" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="DocCollectionOne" sheetId="1" r:id="rId1"/>
-    <sheet name=".lists" sheetId="7" r:id="rId2"/>
+    <sheet name="DocCollection1" sheetId="1" r:id="rId1"/>
+    <sheet name="DocCollection2" sheetId="8" r:id="rId2"/>
+    <sheet name="DocCollection3" sheetId="9" r:id="rId3"/>
+    <sheet name="EdgeCollection1" sheetId="11" r:id="rId4"/>
+    <sheet name=".Graph1" sheetId="14" r:id="rId5"/>
+    <sheet name=".EdgeCollection2" sheetId="12" r:id="rId6"/>
+    <sheet name=".lists" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="DataTypeList">'.lists'!$A$2:$A$8</definedName>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="88">
   <si>
     <t>passwordHash</t>
   </si>
@@ -68,9 +73,6 @@
     <t>json</t>
   </si>
   <si>
-    <t>graphs</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -144,6 +146,168 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>dc2-1</t>
+  </si>
+  <si>
+    <t>dc2-2</t>
+  </si>
+  <si>
+    <t>dc3-3</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>createAt</t>
+  </si>
+  <si>
+    <t>graph-start-1</t>
+  </si>
+  <si>
+    <t>graph-start-2</t>
+  </si>
+  <si>
+    <t>graph-start-3</t>
+  </si>
+  <si>
+    <t>graph-intermediate-1</t>
+  </si>
+  <si>
+    <t>graph-intermediate-2</t>
+  </si>
+  <si>
+    <t>graph-intermediate-3</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Test all datatypes in arango DB. Docs in the collection served as starting nodes in our  test graph</t>
+  </si>
+  <si>
+    <t>Docs in the collection serve as intermediary nodes in our  test graph</t>
+  </si>
+  <si>
+    <t>Docs in the collection serve as terminating nodes in our  test graph</t>
+  </si>
+  <si>
+    <t>dc3-1</t>
+  </si>
+  <si>
+    <t>dc3-2</t>
+  </si>
+  <si>
+    <t>_from</t>
+  </si>
+  <si>
+    <t>_to</t>
+  </si>
+  <si>
+    <t>ec1-1</t>
+  </si>
+  <si>
+    <t>ec2-2</t>
+  </si>
+  <si>
+    <t>graph-terminate-1</t>
+  </si>
+  <si>
+    <t>graph-terminate-2</t>
+  </si>
+  <si>
+    <t>graph-terminate-3</t>
+  </si>
+  <si>
+    <t>G-MIDDLE</t>
+  </si>
+  <si>
+    <t>G-START</t>
+  </si>
+  <si>
+    <t>G-END</t>
+  </si>
+  <si>
+    <t>DocCollection1/dc1-1</t>
+  </si>
+  <si>
+    <t>G-LEG-1</t>
+  </si>
+  <si>
+    <t>Edges in the collection serve as  edges from collection1 to collection 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> type</t>
+  </si>
+  <si>
+    <t>ec2-1</t>
+  </si>
+  <si>
+    <t>ec1-2</t>
+  </si>
+  <si>
+    <t>ec1-3</t>
+  </si>
+  <si>
+    <t>ec2-3</t>
+  </si>
+  <si>
+    <t>ec2-4</t>
+  </si>
+  <si>
+    <t>ec2-5</t>
+  </si>
+  <si>
+    <t>G-LEG-2</t>
+  </si>
+  <si>
+    <t>DocCollection2/dc2-1</t>
+  </si>
+  <si>
+    <t>DocCollection2/dc2-2</t>
+  </si>
+  <si>
+    <t>DocCollection2/dc2-3</t>
+  </si>
+  <si>
+    <t>DocCollection3/dc3-1</t>
+  </si>
+  <si>
+    <t>DocCollection3/dc3-2</t>
+  </si>
+  <si>
+    <t>DocCollection3/dc3-3</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>C1D1 -&gt; C2*</t>
+  </si>
+  <si>
+    <t>dc2-3</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>DocCollection1</t>
+  </si>
+  <si>
+    <t>DocCollection2</t>
+  </si>
+  <si>
+    <t>fromCollections</t>
+  </si>
+  <si>
+    <t>toCollections</t>
+  </si>
+  <si>
+    <t>DocCollection3</t>
   </si>
 </sst>
 </file>
@@ -196,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -204,13 +368,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -238,6 +440,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,222 +757,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="21.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1"/>
+    <col min="1" max="3" width="15.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="21.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1">
+        <v>88</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>40848</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1">
+        <v>99</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="G8" s="7">
+        <v>41255</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2">
-        <v>88</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8">
-        <v>40848</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2">
-        <v>99</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2" t="b">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1">
+        <v>222</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="8">
-        <v>41255</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2">
-        <v>111</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="G9" s="7">
+        <v>36892</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>36892</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D9" s="3"/>
-      <c r="E9" s="8"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D10" s="3"/>
-      <c r="E10" s="8"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-      <c r="E11" s="8"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="E12" s="11"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="10"/>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E10" s="2"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E11" s="2"/>
+      <c r="F11" s="7"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E12" s="2"/>
+      <c r="F12" s="7"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="F13" s="10"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E14" s="2"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E16" s="2"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="9"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:J5" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:H5 B2" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C3 A6:J6" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{9D944A17-348B-2D41-9A48-E3B02CE6F37B}">
@@ -780,65 +1027,873 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCF2433-1C26-0C43-8A34-52888F2E6BE4}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>44822</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{B161CFA1-135B-6D49-B5CC-F61B2F9AF6D2}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:E6 B2:B3" xr:uid="{BF2B3865-DF15-B24D-A601-878E83F24658}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G6" xr:uid="{E34B6D38-0ACC-7449-9411-B684E60C1323}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D69BDD-48F5-1245-8B3A-149AD4BE0AAC}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>45554</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>45554</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>45554</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G6" xr:uid="{41222D5A-5662-694F-844D-BE04CA29514E}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:E6 B2:B3" xr:uid="{5120B4F6-C601-3140-B7F8-CE6CDD60D0E4}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{76C32FC5-0C64-BE40-8599-8439B3EDEE26}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6081FBB0-DD45-E143-A59A-BFD854210439}">
+  <dimension ref="A1:E1048576"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="8"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="8"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="8"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="1048576" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E1048576" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{45421B7B-29D7-AC45-841A-41B842309904}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 A6:E6" xr:uid="{178F24EF-6D92-D545-8CE5-FA6A9C64728F}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6" xr:uid="{480E8F86-FB3B-364F-AE37-38E7D49BB503}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED3B9E3-A274-964C-8725-70593E2BC863}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{01FC2C3A-24DC-3F43-B4F6-24A4705AF1EE}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 B2:B3" xr:uid="{0D0E44B8-B565-4F47-8E2B-2D9F888555BB}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D611DF6E-379A-0F4C-A9ED-39C07B522875}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:F6" xr:uid="{FF2A09C6-3AF7-8140-A380-4475D17A1CAE}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 A6:D6" xr:uid="{0015496E-6437-F341-990B-EBAAB161F1C1}">
+      <formula1>DataTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{067EF2D7-458D-CB4F-847A-741EA0CDC7D2}">
+      <formula1>WorksheetTypeList</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D39D9E3-0EB2-BA4D-9DA7-B5A172AB8C82}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E1" sqref="E1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
+      <c r="A8" s="13" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc and edge loading complete
</commit_message>
<xml_diff>
--- a/packages/arango/tests/test-arango-data-loading.xlsx
+++ b/packages/arango/tests/test-arango-data-loading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/arango/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E2A248-6401-214B-9865-97AB3D684A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3EDA4A-DEAA-CC4E-B37E-8F912D23F447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38580" yWindow="6440" windowWidth="31600" windowHeight="18940" activeTab="5" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="2980" yWindow="2300" windowWidth="27760" windowHeight="24000" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="DocCollection1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="DocCollection3" sheetId="9" r:id="rId3"/>
     <sheet name="EdgeCollection1" sheetId="11" r:id="rId4"/>
     <sheet name=".EdgeCollection2" sheetId="12" r:id="rId5"/>
-    <sheet name=".Graph1" sheetId="14" r:id="rId6"/>
+    <sheet name="Graph1" sheetId="14" r:id="rId6"/>
     <sheet name=".iists" sheetId="15" r:id="rId7"/>
   </sheets>
   <definedNames>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="102">
   <si>
     <t>passwordHash</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>ArangoTypes</t>
+  </si>
+  <si>
+    <t>dataLayout</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -409,11 +412,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -443,6 +472,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,161 +808,137 @@
     <col min="8" max="8" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="E7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="1">
-        <v>88</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>40848</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="1">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="7">
-        <v>41255</v>
+        <v>40848</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>17</v>
@@ -935,41 +946,67 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D9" s="1">
-        <v>222</v>
+        <v>99</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="7">
-        <v>36892</v>
+        <v>41255</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E10" s="2"/>
-      <c r="F10" s="7"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="1">
+        <v>222</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>36892</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E11" s="2"/>
@@ -981,53 +1018,59 @@
       <c r="E12" s="2"/>
       <c r="F12" s="7"/>
       <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="7"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E14" s="2"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="F14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="E15" s="2"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E16" s="2"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="9"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
       <formula1>DataTypeList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{9D944A17-348B-2D41-9A48-E3B02CE6F37B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{9D944A17-348B-2D41-9A48-E3B02CE6F37B}">
       <formula1>ArangoTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{0983B12D-A66C-D343-AA0A-AF0607FD755D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{0983B12D-A66C-D343-AA0A-AF0607FD755D}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:J6" xr:uid="{F5EBDFFC-CEB8-844D-82B6-30A688D6A457}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:J7" xr:uid="{F5EBDFFC-CEB8-844D-82B6-30A688D6A457}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{B0E2AB6E-4345-9B41-B887-A598C04382B8}">
-      <formula1>ArangoTypes</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{53A585E2-96AC-D24B-B678-34F3D5FC505D}">
+      <formula1>DataLayouts</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1037,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCF2433-1C26-0C43-8A34-52888F2E6BE4}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,126 +1094,130 @@
     <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7">
-        <v>45553</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="7">
-        <v>45187</v>
+        <v>45553</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1" t="b">
+      <c r="D10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E10" s="7">
         <v>44822</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="2"/>
-      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" s="2"/>
@@ -1181,36 +1228,43 @@
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="2"/>
+      <c r="A14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="2"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:E6" xr:uid="{BF2B3865-DF15-B24D-A601-878E83F24658}">
+  <dataValidations disablePrompts="1" count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:E7" xr:uid="{BF2B3865-DF15-B24D-A601-878E83F24658}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G6" xr:uid="{E34B6D38-0ACC-7449-9411-B684E60C1323}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G7" xr:uid="{E34B6D38-0ACC-7449-9411-B684E60C1323}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{C0BFDD26-DA60-C34F-A268-80F0A898DB77}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{C0BFDD26-DA60-C34F-A268-80F0A898DB77}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{96C218C7-E28A-A848-A062-D0D4A1513624}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{96C218C7-E28A-A848-A062-D0D4A1513624}">
       <formula1>ArangoTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{458A44DF-1C36-C046-9F91-534989E4EBAF}">
+      <formula1>DataLayouts</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1220,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D69BDD-48F5-1245-8B3A-149AD4BE0AAC}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1234,98 +1288,89 @@
     <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7">
-        <v>45554</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="b">
         <v>1</v>
@@ -1336,13 +1381,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="b">
         <v>1</v>
@@ -1352,8 +1397,21 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="2"/>
-      <c r="E10" s="7"/>
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>45554</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" s="2"/>
@@ -1364,36 +1422,43 @@
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="2"/>
+      <c r="A14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="2"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G6" xr:uid="{41222D5A-5662-694F-844D-BE04CA29514E}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G7" xr:uid="{41222D5A-5662-694F-844D-BE04CA29514E}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:E6" xr:uid="{5120B4F6-C601-3140-B7F8-CE6CDD60D0E4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:E7" xr:uid="{5120B4F6-C601-3140-B7F8-CE6CDD60D0E4}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{A7E57C84-4D99-5042-9559-ACECC86170C0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{A7E57C84-4D99-5042-9559-ACECC86170C0}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0EBDBAF7-9C44-2545-8EC7-E27EBC3940DF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{0EBDBAF7-9C44-2545-8EC7-E27EBC3940DF}">
       <formula1>ArangoTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{2314E17E-B2B5-074F-9ABE-DF2536AADA8C}">
+      <formula1>DataLayouts</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1403,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6081FBB0-DD45-E143-A59A-BFD854210439}">
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1417,98 +1482,89 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>78</v>
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>61</v>
@@ -1519,13 +1575,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>61</v>
@@ -1535,8 +1591,21 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="8"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="8"/>
@@ -1547,37 +1616,41 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
       <c r="C13" s="8"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="2"/>
+      <c r="A14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="2"/>
-    </row>
-    <row r="1048576" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1048576" s="1"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:E6" xr:uid="{178F24EF-6D92-D545-8CE5-FA6A9C64728F}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:E7" xr:uid="{178F24EF-6D92-D545-8CE5-FA6A9C64728F}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6" xr:uid="{480E8F86-FB3B-364F-AE37-38E7D49BB503}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7" xr:uid="{480E8F86-FB3B-364F-AE37-38E7D49BB503}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{DD1ACA4B-48ED-6240-8842-FB4CDDDA8208}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{DD1ACA4B-48ED-6240-8842-FB4CDDDA8208}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{A7BE1025-3ACE-9240-8F55-8985FEDC73E1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{A7BE1025-3ACE-9240-8F55-8985FEDC73E1}">
       <formula1>ArangoTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{DDED2FB5-5CB2-4743-B45E-01C236B9355E}">
+      <formula1>DataLayouts</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1587,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D611DF6E-379A-0F4C-A9ED-39C07B522875}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1601,89 +1674,83 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>70</v>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>70</v>
@@ -1691,13 +1758,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>70</v>
@@ -1705,13 +1772,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>70</v>
@@ -1719,50 +1786,67 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D14" s="2"/>
+      <c r="A14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D16" s="2"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:F6" xr:uid="{FF2A09C6-3AF7-8140-A380-4475D17A1CAE}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:F7" xr:uid="{FF2A09C6-3AF7-8140-A380-4475D17A1CAE}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:D6" xr:uid="{0015496E-6437-F341-990B-EBAAB161F1C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:D7" xr:uid="{0015496E-6437-F341-990B-EBAAB161F1C1}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{D9C65762-A217-0B43-B32D-653C338E5E57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{D9C65762-A217-0B43-B32D-653C338E5E57}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{4CFA3202-F0F0-C547-8518-8DC309F8C9F9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{4CFA3202-F0F0-C547-8518-8DC309F8C9F9}">
       <formula1>ArangoTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{8C5A924B-C744-C74F-8A27-2141D43EFC2B}">
+      <formula1>DataLayouts</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1772,10 +1856,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED3B9E3-A274-964C-8725-70593E2BC863}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1785,75 +1869,87 @@
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
         <v>82</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 B5:B6" xr:uid="{4ABA0D2C-8A95-C244-90F8-D71B3CC003A5}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4 B6:B7" xr:uid="{4ABA0D2C-8A95-C244-90F8-D71B3CC003A5}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{77AA1E3D-24F3-FE42-9110-B5F8B57525AA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{77AA1E3D-24F3-FE42-9110-B5F8B57525AA}">
       <formula1>ArangoTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{C5C6152D-72C9-7948-B0F8-1DB6471D0E55}">
+      <formula1>DataLayouts</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
get scaffolding in place for graph loading
</commit_message>
<xml_diff>
--- a/packages/arango/tests/test-arango-data-loading.xlsx
+++ b/packages/arango/tests/test-arango-data-loading.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/arango/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3EDA4A-DEAA-CC4E-B37E-8F912D23F447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8B04D8-92C1-8B49-934F-F0954959E7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="2300" windowWidth="27760" windowHeight="24000" activeTab="3" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="25080" yWindow="1700" windowWidth="27760" windowHeight="24000" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="DocCollection1" sheetId="1" r:id="rId1"/>
     <sheet name="DocCollection2" sheetId="8" r:id="rId2"/>
     <sheet name="DocCollection3" sheetId="9" r:id="rId3"/>
     <sheet name="EdgeCollection1" sheetId="11" r:id="rId4"/>
-    <sheet name=".EdgeCollection2" sheetId="12" r:id="rId5"/>
+    <sheet name="EdgeCollection2" sheetId="12" r:id="rId5"/>
     <sheet name="Graph1" sheetId="14" r:id="rId6"/>
     <sheet name=".iists" sheetId="15" r:id="rId7"/>
   </sheets>
@@ -1470,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6081FBB0-DD45-E143-A59A-BFD854210439}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D611DF6E-379A-0F4C-A9ED-39C07B522875}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
78 arrango data loader (#142)
* minor naming changes

* Improve option defintion and handling for getDG and createDB

* convert db optoins from enum to strings

* update arango data loader to use new db enum defs

* minor cleanup

* convert enums to string ... goodby enums

* doc and edge loading complete

* graph additions checkpoint

* get scaffolding in place for graph loading

* Improve name DataList -> DataCollectoion

* support termination delimeters

* hate to commit here, funky state, but I need to capture a base upon which to evolve a new idea

* funk check point

* Fiiiiinallly got collection parsing done

* minor tweaks

* update arangojs

* xpoint

* update all npm packages

* add graph creation

* publish new versions of arango and spreadsheet-parser
</commit_message>
<xml_diff>
--- a/packages/arango/tests/test-arango-data-loading.xlsx
+++ b/packages/arango/tests/test-arango-data-loading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland/packages/arango/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/sentosa/code/stcland-arango/packages/arango/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE61001-BABA-724B-8B85-3F10DDB14843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EAFE4B-64E0-1245-9859-196E809A2087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60300" yWindow="2760" windowWidth="34560" windowHeight="19960" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
+    <workbookView xWindow="71500" yWindow="2900" windowWidth="28480" windowHeight="22800" activeTab="4" xr2:uid="{A9FAF7F1-B5C0-2C48-9AE9-611ABBBDB9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="DocCollection1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="EdgeCollection1" sheetId="11" r:id="rId4"/>
     <sheet name="EdgeCollection2" sheetId="12" r:id="rId5"/>
     <sheet name="Graph1" sheetId="14" r:id="rId6"/>
-    <sheet name=".iists" sheetId="15" r:id="rId7"/>
+    <sheet name=".Graph2" sheetId="17" r:id="rId7"/>
+    <sheet name=".iists" sheetId="15" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="ArangoTypes">'.iists'!$A$2:$A$4</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="107">
   <si>
     <t>passwordHash</t>
   </si>
@@ -141,9 +142,6 @@
     <t>{ "array": [ "in", "an", "object" ]}</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>dc2-1</t>
   </si>
   <si>
@@ -192,24 +190,12 @@
     <t>ec2-2</t>
   </si>
   <si>
-    <t>G-MIDDLE</t>
-  </si>
-  <si>
-    <t>G-START</t>
-  </si>
-  <si>
-    <t>G-END</t>
-  </si>
-  <si>
     <t>DocCollection1/dc1-1</t>
   </si>
   <si>
     <t>G-LEG-1</t>
   </si>
   <si>
-    <t>Edges in the collection serve as  edges from collection1 to collection 2</t>
-  </si>
-  <si>
     <t xml:space="preserve"> type</t>
   </si>
   <si>
@@ -240,9 +226,6 @@
     <t>DocCollection2/dc2-2</t>
   </si>
   <si>
-    <t>DocCollection2/dc2-3</t>
-  </si>
-  <si>
     <t>DocCollection3/dc3-1</t>
   </si>
   <si>
@@ -255,9 +238,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>C1D1 -&gt; C2*</t>
-  </si>
-  <si>
     <t>dc2-3</t>
   </si>
   <si>
@@ -288,9 +268,6 @@
     <t>dataTable</t>
   </si>
   <si>
-    <t>dataList</t>
-  </si>
-  <si>
     <t>frontMatterOnly</t>
   </si>
   <si>
@@ -336,40 +313,61 @@
     <t>g-start-3</t>
   </si>
   <si>
-    <t>g-intermediate-1</t>
-  </si>
-  <si>
-    <t>gr-intermediate-2</t>
-  </si>
-  <si>
-    <t>g-intermediate-3</t>
-  </si>
-  <si>
-    <t>g1</t>
-  </si>
-  <si>
-    <t>graphName</t>
-  </si>
-  <si>
-    <t>Test graph 1 using all collections</t>
-  </si>
-  <si>
     <t>dc3-4</t>
   </si>
   <si>
-    <t>g-terminate-1</t>
-  </si>
-  <si>
-    <t>g-terminate-2</t>
-  </si>
-  <si>
-    <t>g-terminate-3</t>
-  </si>
-  <si>
-    <t>ec1-4</t>
-  </si>
-  <si>
-    <t>C1D1 -&gt; C3D1</t>
+    <t>dataCollection</t>
+  </si>
+  <si>
+    <t>Test graphs</t>
+  </si>
+  <si>
+    <t>DocCollection1/dc1-2</t>
+  </si>
+  <si>
+    <t>dc3-5</t>
+  </si>
+  <si>
+    <t>Edges in the collection serve as  edges from collection1 to collections 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Edges in the collection serve as  edges from collection 2 to collection 3</t>
+  </si>
+  <si>
+    <t>11 -&gt; 31</t>
+  </si>
+  <si>
+    <t>11 -&gt; 21</t>
+  </si>
+  <si>
+    <t>12- &gt; 22</t>
+  </si>
+  <si>
+    <t>21 -&gt; 32</t>
+  </si>
+  <si>
+    <t>21 -&gt; 33</t>
+  </si>
+  <si>
+    <t>21 -&gt; 34</t>
+  </si>
+  <si>
+    <t>DocCollection3/dc3-4</t>
+  </si>
+  <si>
+    <t>22 -&gt; 33</t>
+  </si>
+  <si>
+    <t>22 -&gt; 34</t>
+  </si>
+  <si>
+    <t>EdgeCollection1</t>
+  </si>
+  <si>
+    <t>EdgeCollection2</t>
+  </si>
+  <si>
+    <t>Graph 1</t>
   </si>
 </sst>
 </file>
@@ -810,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B101DD8F-9A36-0342-BC29-1E3C3A22B2B5}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,22 +824,22 @@
     <col min="8" max="8" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -850,55 +848,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="G6" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="H6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -906,156 +901,144 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="G7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="H7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="1">
+        <v>85</v>
+      </c>
+      <c r="C8" s="1">
         <v>88</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="1" t="b">
+      <c r="E8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G8" s="7">
+      <c r="F8" s="7">
         <v>40848</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H8" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="1">
+        <v>86</v>
+      </c>
+      <c r="C9" s="1">
         <v>99</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1" t="b">
+      <c r="E9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="7">
+      <c r="F9" s="7">
         <v>41255</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="1">
+        <v>87</v>
+      </c>
+      <c r="C10" s="1">
         <v>222</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="1" t="b">
+      <c r="E10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="7">
+      <c r="F10" s="7">
         <v>36892</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E11" s="2"/>
       <c r="F11" s="7"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E12" s="2"/>
       <c r="F12" s="7"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E13" s="2"/>
       <c r="F13" s="7"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="D14" s="8"/>
       <c r="F14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E15" s="2"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1072,7 +1055,7 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7" xr:uid="{A7427D63-E072-9D43-B99E-939C11A4ABCC}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{FB632601-5BD8-4B42-ACD7-4B96F03BA7D3}">
@@ -1084,11 +1067,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{0983B12D-A66C-D343-AA0A-AF0607FD755D}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:J7" xr:uid="{F5EBDFFC-CEB8-844D-82B6-30A688D6A457}">
-      <formula1>TableDataTypes</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{53A585E2-96AC-D24B-B678-34F3D5FC505D}">
       <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:I7" xr:uid="{F5EBDFFC-CEB8-844D-82B6-30A688D6A457}">
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1101,7 +1084,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,10 +1097,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1127,7 +1110,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1138,13 +1121,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1157,16 +1140,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1174,68 +1151,50 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="1" t="b">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="7">
+      <c r="C8" s="7">
         <v>45553</v>
       </c>
+      <c r="D8"/>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="1" t="b">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E9" s="7">
+      <c r="C9" s="7">
         <v>45187</v>
       </c>
+      <c r="D9"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="1" t="b">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="7">
+      <c r="C10" s="7">
         <v>44822</v>
       </c>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" s="2"/>
@@ -1269,10 +1228,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:E7" xr:uid="{BF2B3865-DF15-B24D-A601-878E83F24658}">
-      <formula1>TableDataTypes</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G7" xr:uid="{E34B6D38-0ACC-7449-9411-B684E60C1323}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7" xr:uid="{E34B6D38-0ACC-7449-9411-B684E60C1323}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{C0BFDD26-DA60-C34F-A268-80F0A898DB77}">
@@ -1283,6 +1239,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{458A44DF-1C36-C046-9F91-534989E4EBAF}">
       <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:C7" xr:uid="{BF2B3865-DF15-B24D-A601-878E83F24658}">
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1295,7 +1254,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1308,10 +1267,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1321,7 +1280,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1332,13 +1291,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1351,16 +1310,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1368,89 +1321,76 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="1" t="b">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="7">
+      <c r="C8" s="7">
         <v>45554</v>
       </c>
+      <c r="D8"/>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="1" t="b">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="C9" s="7">
         <v>45554</v>
       </c>
+      <c r="D9"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="1" t="b">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="7">
+      <c r="C10" s="7">
         <v>45554</v>
       </c>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="1" t="b">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="7">
+      <c r="C11" s="7">
         <v>45554</v>
       </c>
+      <c r="D11"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="2"/>
-      <c r="E12" s="7"/>
+      <c r="A12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>45554</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="2"/>
@@ -1476,11 +1416,8 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:G7" xr:uid="{41222D5A-5662-694F-844D-BE04CA29514E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7" xr:uid="{41222D5A-5662-694F-844D-BE04CA29514E}">
       <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:E7" xr:uid="{5120B4F6-C601-3140-B7F8-CE6CDD60D0E4}">
-      <formula1>TableDataTypes</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{A7E57C84-4D99-5042-9559-ACECC86170C0}">
       <formula1>ListDataTypes</formula1>
@@ -1490,6 +1427,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{2314E17E-B2B5-074F-9ABE-DF2536AADA8C}">
       <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:C7" xr:uid="{5120B4F6-C601-3140-B7F8-CE6CDD60D0E4}">
+      <formula1>TableDataTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1502,7 +1442,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1516,10 +1456,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1529,7 +1469,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1540,13 +1480,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1559,16 +1499,16 @@
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1590,71 +1530,58 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="C11" s="8"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" s="8"/>
@@ -1705,10 +1632,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D611DF6E-379A-0F4C-A9ED-39C07B522875}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1719,22 +1646,22 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1743,136 +1670,151 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>60</v>
-      </c>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1883,10 +1825,10 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:F7" xr:uid="{FF2A09C6-3AF7-8140-A380-4475D17A1CAE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7" xr:uid="{FF2A09C6-3AF7-8140-A380-4475D17A1CAE}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:D7" xr:uid="{0015496E-6437-F341-990B-EBAAB161F1C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:E7" xr:uid="{0015496E-6437-F341-990B-EBAAB161F1C1}">
       <formula1>TableDataTypes</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{D9C65762-A217-0B43-B32D-653C338E5E57}">
@@ -1906,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED3B9E3-A274-964C-8725-70593E2BC863}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1921,10 +1863,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1936,70 +1878,113 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
+      <c r="A5" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B5 B7:B8" xr:uid="{4ABA0D2C-8A95-C244-90F8-D71B3CC003A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B8 B3:B4 B11:B12" xr:uid="{4ABA0D2C-8A95-C244-90F8-D71B3CC003A5}">
       <formula1>ListDataTypes</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{77AA1E3D-24F3-FE42-9110-B5F8B57525AA}">
@@ -2015,11 +2000,165 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2A6C47-EC5A-B44C-A752-C5B304789AE5}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{8EC616BF-AC33-E043-984A-6A3C68224DC8}">
+      <formula1>DataLayouts</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{5AF9A0A2-B948-3D41-B1AC-B762EC654862}">
+      <formula1>ArangoTypes</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B8 B3:B4 B11:B12" xr:uid="{3F0360AD-C57E-E44F-A3D2-793815F9E0BC}">
+      <formula1>ListDataTypes</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E4564F-11AA-3F4C-8351-EC1CFA461E28}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2029,16 +2168,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2052,7 +2191,7 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2066,12 +2205,12 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -2080,7 +2219,7 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2117,37 +2256,37 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>